<commit_message>
Ajuste no Orcamento inicial do projeto com telefonia
</commit_message>
<xml_diff>
--- a/PastaDocumentos/Orcamento.xlsx
+++ b/PastaDocumentos/Orcamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonrmlocal\Downloads\ExemploGitFlow\2TDSS-ExemploGit-2024\PastaDocumentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A979B1-7F56-4B54-8CE5-66B36DA4319F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D270573-3EC8-4B06-B071-EE4DFD935F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -375,7 +375,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +410,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>34</v>
+        <v>340000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>